<commit_message>
Se añadió interpolación y ruido a los datos de carga del edificio.
</commit_message>
<xml_diff>
--- a/simulation/data.xlsx
+++ b/simulation/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b2d34e98eeaf6352/Documentos/GitHub/case-simulation/simulation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="8_{BF067246-BF08-0D40-88F5-9E2D9C934D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC6421C3-59BA-4ED0-8A02-ED4AE3FF24E1}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="8_{BF067246-BF08-0D40-88F5-9E2D9C934D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9997FAEB-E9CF-449E-A996-419A949AD502}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C377CCAD-6F87-EB40-9FE3-7C22EAD05773}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Fecha/Hora</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>Carga (pu)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1022,6 +1019,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -1319,10 +1320,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{469A3634-ECA2-EA4C-9305-A0A3706F9F5D}">
-  <dimension ref="A1:L8761"/>
+  <dimension ref="A1:C8761"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1506,7 +1507,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>40909.625</v>
       </c>
@@ -1517,7 +1518,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>40909.666666666664</v>
       </c>
@@ -1528,7 +1529,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>40909.708333333336</v>
       </c>
@@ -1539,7 +1540,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>40909.75</v>
       </c>
@@ -1550,7 +1551,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>40909.791666666664</v>
       </c>
@@ -1561,7 +1562,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>40909.833333333336</v>
       </c>
@@ -1572,7 +1573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>40909.875</v>
       </c>
@@ -1583,7 +1584,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>40909.916666666664</v>
       </c>
@@ -1594,7 +1595,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>40909.958333333336</v>
       </c>
@@ -1604,35 +1605,32 @@
       <c r="C25">
         <v>0.4</v>
       </c>
-      <c r="L25" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="1"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="1"/>
     </row>

</xml_diff>